<commit_message>
Add levels up to 50
</commit_message>
<xml_diff>
--- a/levels/level1.xlsx
+++ b/levels/level1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Projects\mobgenerator_weaponswitcher\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBCA316-2367-4856-BADA-DFEEAC332CD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40D3BB5-E4C9-4F13-806B-4EAD595D39AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="37470" windowHeight="21840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>deltaTime</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>all enemies:</t>
+  </si>
+  <si>
+    <t>EnemyPrefabs/Bullet Enemies/Neo Fly/Neo Fly</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,39 +500,33 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
       <c r="E1">
         <f>meta!$B$1*ROW()</f>
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
       <c r="E2">
         <f>meta!$B$1*ROW()</f>
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3">
         <f>meta!$B$1*ROW()</f>
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="E4">
         <f>meta!$B$1*ROW()</f>
         <v>12</v>
@@ -537,10 +534,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f>meta!$B$1*ROW()</f>
@@ -554,6 +548,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="E7">
         <f>meta!$B$1*ROW()</f>
         <v>21</v>
@@ -563,20 +560,14 @@
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
       <c r="E8">
         <f>meta!$B$1*ROW()</f>
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>2</v>
+      <c r="D9">
+        <v>7</v>
       </c>
       <c r="E9">
         <f>meta!$B$1*ROW()</f>
@@ -596,12 +587,6 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
       <c r="E12">
         <f>meta!$B$1*ROW()</f>
         <v>36</v>
@@ -620,12 +605,6 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>6</v>
-      </c>
       <c r="E15">
         <f>meta!$B$1*ROW()</f>
         <v>45</v>
@@ -637,103 +616,97 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17">
         <f>meta!$B$1*ROW()</f>
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18">
         <f>meta!$B$1*ROW()</f>
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19">
         <f>meta!$B$1*ROW()</f>
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20">
         <f>meta!$B$1*ROW()</f>
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21">
         <f>meta!$B$1*ROW()</f>
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E22">
         <f>meta!$B$1*ROW()</f>
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E23">
         <f>meta!$B$1*ROW()</f>
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E24">
         <f>meta!$B$1*ROW()</f>
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E25">
         <f>meta!$B$1*ROW()</f>
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E26">
         <f>meta!$B$1*ROW()</f>
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E27">
         <f>meta!$B$1*ROW()</f>
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E28">
         <f>meta!$B$1*ROW()</f>
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E29">
         <f>meta!$B$1*ROW()</f>
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E30">
         <f>meta!$B$1*ROW()</f>
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E31">
         <f>meta!$B$1*ROW()</f>
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E32">
         <f>meta!$B$1*ROW()</f>
         <v>96</v>
@@ -843,10 +816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,6 +980,26 @@
       </c>
       <c r="G7" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>